<commit_message>
BATAU - Template Update Category KPIs
</commit_message>
<xml_diff>
--- a/Projects/BATAU_SAND/Data/Template.xlsx
+++ b/Projects/BATAU_SAND/Data/Template.xlsx
@@ -440,23 +440,23 @@
   <dimension ref="1:27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.2914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.6882591093117"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2753036437247"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="69.9352226720648"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.6801619433198"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="47.5546558704454"/>
-    <col collapsed="false" hidden="false" max="1020" min="11" style="2" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="70.4858299595142"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="2" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,7 +1303,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>54</v>
@@ -1345,13 +1345,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.0202429149798"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.663967611336"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.53441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>